<commit_message>
Test cds api, issue persists
</commit_message>
<xml_diff>
--- a/Parameters/weather_parameters.xlsx
+++ b/Parameters/weather_parameters.xlsx
@@ -46,7 +46,7 @@
     <t>Filename</t>
   </si>
   <si>
-    <t>Laos23</t>
+    <t>EU23</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>100.0833</v>
+        <v>-10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -460,7 +460,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>107.6333</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -468,7 +468,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>13.9197</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -476,7 +476,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>22.5</v>
+        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">

</xml_diff>